<commit_message>
RTU1S and VAV1.1 have been written
</commit_message>
<xml_diff>
--- a/assets/List_AllInputs.xlsx
+++ b/assets/List_AllInputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coals01826\Desktop\Coding\hanson-bas\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schra02155\PycharmProjects\hanson-bas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646E5B4-1F12-4CA2-8594-9E59B883441C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D977591-8586-4702-92AD-2CDFF80DAC63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$463</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1200,7 +1211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1598,13 +1609,13 @@
   <dimension ref="A1:S463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -1627,7 +1638,7 @@
     <col min="19" max="19" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>246</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1796,7 +1807,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1943,7 +1954,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1989,7 +2000,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2035,7 +2046,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2130,7 +2141,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2182,7 +2193,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2231,7 +2242,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2280,7 +2291,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2378,7 +2389,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2485,7 +2496,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2540,7 +2551,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2589,7 +2600,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2635,7 +2646,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2690,7 +2701,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2745,7 +2756,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2797,7 +2808,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2846,7 +2857,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2947,7 +2958,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2996,7 +3007,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3045,7 +3056,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3091,7 +3102,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3137,7 +3148,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="1"/>
       <c r="C31" t="s">
         <v>374</v>
@@ -3167,7 +3178,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="1"/>
       <c r="C32" t="s">
         <v>375</v>
@@ -3197,7 +3208,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" s="1"/>
       <c r="C33" t="s">
         <v>364</v>
@@ -3227,7 +3238,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" s="1"/>
       <c r="C34" t="s">
         <v>365</v>
@@ -3257,7 +3268,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" s="1"/>
       <c r="C35" t="s">
         <v>44</v>
@@ -3287,7 +3298,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" s="1"/>
       <c r="C36" t="s">
         <v>376</v>
@@ -3314,7 +3325,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" s="1"/>
       <c r="C37" t="s">
         <v>377</v>
@@ -3341,7 +3352,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" s="1"/>
       <c r="C38" t="s">
         <v>366</v>
@@ -3368,7 +3379,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
         <v>367</v>
@@ -3395,7 +3406,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
         <v>378</v>
@@ -3422,7 +3433,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="C41" t="s">
         <v>379</v>
       </c>
@@ -3435,6 +3446,9 @@
       <c r="F41" t="s">
         <v>250</v>
       </c>
+      <c r="I41">
+        <v>1000</v>
+      </c>
       <c r="J41" t="s">
         <v>15</v>
       </c>
@@ -3442,7 +3456,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="C42" t="s">
         <v>368</v>
       </c>
@@ -3455,6 +3469,9 @@
       <c r="F42" t="s">
         <v>250</v>
       </c>
+      <c r="I42">
+        <v>1000</v>
+      </c>
       <c r="J42" t="s">
         <v>15</v>
       </c>
@@ -3462,7 +3479,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="C43" t="s">
         <v>380</v>
       </c>
@@ -3488,7 +3505,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="C44" t="s">
         <v>381</v>
       </c>
@@ -3514,7 +3531,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="C45" t="s">
         <v>382</v>
       </c>
@@ -3540,7 +3557,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" s="1">
         <v>29</v>
       </c>
@@ -3592,7 +3609,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" s="1">
         <v>30</v>
       </c>
@@ -3641,7 +3658,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" s="1">
         <v>31</v>
       </c>
@@ -3690,7 +3707,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" s="1">
         <v>32</v>
       </c>
@@ -3736,7 +3753,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" s="1">
         <v>33</v>
       </c>
@@ -3782,7 +3799,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" s="1">
         <v>34</v>
       </c>
@@ -3834,7 +3851,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" s="1">
         <v>35</v>
       </c>
@@ -3883,7 +3900,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="A53" s="1">
         <v>36</v>
       </c>
@@ -3932,7 +3949,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="A54" s="1">
         <v>37</v>
       </c>
@@ -3978,7 +3995,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="A55" s="1">
         <v>38</v>
       </c>
@@ -4033,7 +4050,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="A56" s="1">
         <v>39</v>
       </c>
@@ -4082,7 +4099,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="A57" s="1">
         <v>40</v>
       </c>
@@ -4128,7 +4145,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="A58" s="1">
         <v>41</v>
       </c>
@@ -4177,7 +4194,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="A59" s="1">
         <v>42</v>
       </c>
@@ -4226,7 +4243,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="A60" s="1">
         <v>43</v>
       </c>
@@ -4275,7 +4292,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="A61" s="1">
         <v>44</v>
       </c>
@@ -4327,7 +4344,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="A62" s="1">
         <v>45</v>
       </c>
@@ -4382,7 +4399,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="A63" s="1">
         <v>46</v>
       </c>
@@ -4431,7 +4448,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="A64" s="1">
         <v>47</v>
       </c>
@@ -4477,7 +4494,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65" s="1">
         <v>48</v>
       </c>
@@ -4526,7 +4543,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="A66" s="1">
         <v>49</v>
       </c>
@@ -4572,7 +4589,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="A67" s="1">
         <v>50</v>
       </c>
@@ -4618,7 +4635,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="A68" s="1">
         <v>51</v>
       </c>
@@ -4673,7 +4690,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69" s="1">
         <v>52</v>
       </c>
@@ -4722,7 +4739,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="A70" s="1">
         <v>53</v>
       </c>
@@ -4768,7 +4785,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="A71" s="1">
         <v>54</v>
       </c>
@@ -4823,7 +4840,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72" s="1">
         <v>55</v>
       </c>
@@ -4872,7 +4889,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="A73" s="1">
         <v>56</v>
       </c>
@@ -4921,7 +4938,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="A74" s="1">
         <v>57</v>
       </c>
@@ -4967,7 +4984,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="A75" s="1">
         <v>58</v>
       </c>
@@ -5016,7 +5033,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="A76" s="1">
         <v>59</v>
       </c>
@@ -5065,7 +5082,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77" s="1">
         <v>60</v>
       </c>
@@ -5117,7 +5134,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="A78" s="1">
         <v>61</v>
       </c>
@@ -5166,7 +5183,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="A79" s="1">
         <v>62</v>
       </c>
@@ -5215,7 +5232,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17">
       <c r="A80" s="1">
         <v>63</v>
       </c>
@@ -5261,7 +5278,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17">
       <c r="A81" s="1">
         <v>64</v>
       </c>
@@ -5313,7 +5330,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17">
       <c r="A82" s="1">
         <v>65</v>
       </c>
@@ -5362,7 +5379,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17">
       <c r="A83" s="1">
         <v>66</v>
       </c>
@@ -5411,7 +5428,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17">
       <c r="A84" s="1">
         <v>67</v>
       </c>
@@ -5457,7 +5474,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17">
       <c r="A85" s="1">
         <v>68</v>
       </c>
@@ -5509,7 +5526,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17">
       <c r="A86" s="1">
         <v>69</v>
       </c>
@@ -5558,7 +5575,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17">
       <c r="A87" s="1">
         <v>70</v>
       </c>
@@ -5607,7 +5624,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17">
       <c r="A88" s="1">
         <v>71</v>
       </c>
@@ -5656,7 +5673,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17">
       <c r="A89" s="1">
         <v>72</v>
       </c>
@@ -5702,7 +5719,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17">
       <c r="A90" s="1">
         <v>73</v>
       </c>
@@ -5754,7 +5771,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17">
       <c r="A91" s="1">
         <v>74</v>
       </c>
@@ -5803,7 +5820,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17">
       <c r="A92" s="1">
         <v>75</v>
       </c>
@@ -5852,7 +5869,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17">
       <c r="A93" s="1">
         <v>76</v>
       </c>
@@ -5901,7 +5918,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17">
       <c r="A94" s="1">
         <v>77</v>
       </c>
@@ -5950,7 +5967,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17">
       <c r="A95" s="1">
         <v>78</v>
       </c>
@@ -5996,7 +6013,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17">
       <c r="A96" s="1">
         <v>79</v>
       </c>
@@ -6051,7 +6068,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="A97" s="1">
         <v>80</v>
       </c>
@@ -6100,7 +6117,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="A98" s="1">
         <v>81</v>
       </c>
@@ -6149,7 +6166,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="A99" s="1">
         <v>82</v>
       </c>
@@ -6195,7 +6212,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17">
       <c r="A100" s="1">
         <v>83</v>
       </c>
@@ -6241,7 +6258,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101" s="1">
         <v>84</v>
       </c>
@@ -6293,7 +6310,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17">
       <c r="A102" s="1">
         <v>85</v>
       </c>
@@ -6342,7 +6359,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17">
       <c r="A103" s="1">
         <v>86</v>
       </c>
@@ -6391,7 +6408,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17">
       <c r="A104" s="1">
         <v>87</v>
       </c>
@@ -6440,7 +6457,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17">
       <c r="A105" s="1">
         <v>88</v>
       </c>
@@ -6486,7 +6503,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17">
       <c r="A106" s="1">
         <v>89</v>
       </c>
@@ -6541,7 +6558,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17">
       <c r="A107" s="1">
         <v>90</v>
       </c>
@@ -6590,7 +6607,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17">
       <c r="A108" s="1">
         <v>91</v>
       </c>
@@ -6636,7 +6653,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17">
       <c r="A109" s="1">
         <v>92</v>
       </c>
@@ -6685,7 +6702,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17">
       <c r="A110" s="1">
         <v>93</v>
       </c>
@@ -6731,7 +6748,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17">
       <c r="A111" s="1">
         <v>94</v>
       </c>
@@ -6786,7 +6803,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17">
       <c r="A112" s="1">
         <v>95</v>
       </c>
@@ -6835,7 +6852,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113" s="1">
         <v>96</v>
       </c>
@@ -6881,7 +6898,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17">
       <c r="A114" s="1">
         <v>97</v>
       </c>
@@ -6930,7 +6947,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="A115" s="1">
         <v>98</v>
       </c>
@@ -6976,7 +6993,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="A116" s="1">
         <v>99</v>
       </c>
@@ -7031,7 +7048,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17">
       <c r="A117" s="1">
         <v>100</v>
       </c>
@@ -7080,7 +7097,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="A118" s="1">
         <v>101</v>
       </c>
@@ -7126,7 +7143,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="A119" s="1">
         <v>102</v>
       </c>
@@ -7181,7 +7198,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
       <c r="A120" s="1">
         <v>103</v>
       </c>
@@ -7230,7 +7247,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17">
       <c r="A121" s="1">
         <v>104</v>
       </c>
@@ -7276,7 +7293,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17">
       <c r="A122" s="1">
         <v>105</v>
       </c>
@@ -7331,7 +7348,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17">
       <c r="A123" s="1">
         <v>106</v>
       </c>
@@ -7380,7 +7397,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17">
       <c r="A124" s="1">
         <v>107</v>
       </c>
@@ -7426,7 +7443,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17">
       <c r="A125" s="1">
         <v>108</v>
       </c>
@@ -7475,7 +7492,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17">
       <c r="A126" s="1">
         <v>109</v>
       </c>
@@ -7521,7 +7538,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17">
       <c r="A127" s="1">
         <v>110</v>
       </c>
@@ -7576,7 +7593,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17">
       <c r="A128" s="1">
         <v>111</v>
       </c>
@@ -7622,7 +7639,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17">
       <c r="A129" s="1">
         <v>112</v>
       </c>
@@ -7671,7 +7688,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17">
       <c r="A130" s="1">
         <v>113</v>
       </c>
@@ -7720,7 +7737,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17">
       <c r="A131" s="1">
         <v>114</v>
       </c>
@@ -7766,7 +7783,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17">
       <c r="A132" s="1">
         <v>115</v>
       </c>
@@ -7821,7 +7838,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17">
       <c r="A133" s="1">
         <v>116</v>
       </c>
@@ -7870,7 +7887,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17">
       <c r="A134" s="1">
         <v>117</v>
       </c>
@@ -7916,7 +7933,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17">
       <c r="A135" s="1">
         <v>118</v>
       </c>
@@ -7965,7 +7982,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17">
       <c r="A136" s="1">
         <v>119</v>
       </c>
@@ -8014,7 +8031,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17">
       <c r="A137" s="1">
         <v>120</v>
       </c>
@@ -8060,7 +8077,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17">
       <c r="A138" s="1">
         <v>121</v>
       </c>
@@ -8112,7 +8129,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17">
       <c r="A139" s="1">
         <v>122</v>
       </c>
@@ -8161,7 +8178,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17">
       <c r="A140" s="1">
         <v>123</v>
       </c>
@@ -8210,7 +8227,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17">
       <c r="A141" s="1">
         <v>124</v>
       </c>
@@ -8265,7 +8282,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17">
       <c r="A142" s="1">
         <v>125</v>
       </c>
@@ -8314,7 +8331,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17">
       <c r="A143" s="1">
         <v>126</v>
       </c>
@@ -8360,7 +8377,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17">
       <c r="A144" s="1">
         <v>127</v>
       </c>
@@ -8409,7 +8426,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17">
       <c r="A145" s="1">
         <v>128</v>
       </c>
@@ -8455,7 +8472,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17">
       <c r="A146" s="1">
         <v>129</v>
       </c>
@@ -8501,7 +8518,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17">
       <c r="A147" s="1">
         <v>130</v>
       </c>
@@ -8556,7 +8573,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17">
       <c r="A148" s="1">
         <v>131</v>
       </c>
@@ -8602,7 +8619,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17">
       <c r="A149" s="1">
         <v>132</v>
       </c>
@@ -8651,7 +8668,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17">
       <c r="A150" s="1">
         <v>133</v>
       </c>
@@ -8700,7 +8717,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17">
       <c r="A151" s="1">
         <v>134</v>
       </c>
@@ -8746,7 +8763,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17">
       <c r="A152" s="1">
         <v>135</v>
       </c>
@@ -8798,7 +8815,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17">
       <c r="A153" s="1">
         <v>136</v>
       </c>
@@ -8847,7 +8864,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17">
       <c r="A154" s="1">
         <v>137</v>
       </c>
@@ -8896,7 +8913,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17">
       <c r="A155" s="1">
         <v>138</v>
       </c>
@@ -8945,7 +8962,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17">
       <c r="A156" s="1">
         <v>139</v>
       </c>
@@ -8994,7 +9011,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17">
       <c r="A157" s="1">
         <v>140</v>
       </c>
@@ -9040,7 +9057,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17">
       <c r="A158" s="1">
         <v>141</v>
       </c>
@@ -9092,7 +9109,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17">
       <c r="A159" s="1">
         <v>142</v>
       </c>
@@ -9141,7 +9158,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17">
       <c r="A160" s="1">
         <v>143</v>
       </c>
@@ -9190,7 +9207,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17">
       <c r="A161" s="1">
         <v>144</v>
       </c>
@@ -9236,7 +9253,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17">
       <c r="A162" s="1">
         <v>145</v>
       </c>
@@ -9291,7 +9308,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17">
       <c r="A163" s="1">
         <v>146</v>
       </c>
@@ -9340,7 +9357,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17">
       <c r="A164" s="1">
         <v>147</v>
       </c>
@@ -9386,7 +9403,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17">
       <c r="A165" s="1">
         <v>148</v>
       </c>
@@ -9435,7 +9452,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17">
       <c r="A166" s="1">
         <v>149</v>
       </c>
@@ -9481,7 +9498,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17">
       <c r="A167" s="1">
         <v>150</v>
       </c>
@@ -9536,7 +9553,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17">
       <c r="A168" s="1">
         <v>151</v>
       </c>
@@ -9585,7 +9602,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17">
       <c r="A169" s="1">
         <v>152</v>
       </c>
@@ -9631,7 +9648,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17">
       <c r="A170" s="1">
         <v>153</v>
       </c>
@@ -9680,7 +9697,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17">
       <c r="A171" s="1">
         <v>154</v>
       </c>
@@ -9726,7 +9743,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17">
       <c r="A172" s="1">
         <v>155</v>
       </c>
@@ -9781,7 +9798,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17">
       <c r="A173" s="1">
         <v>156</v>
       </c>
@@ -9830,7 +9847,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17">
       <c r="A174" s="1">
         <v>157</v>
       </c>
@@ -9876,7 +9893,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17">
       <c r="A175" s="1">
         <v>158</v>
       </c>
@@ -9925,7 +9942,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17">
       <c r="A176" s="1">
         <v>159</v>
       </c>
@@ -9971,7 +9988,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17">
       <c r="A177" s="1">
         <v>160</v>
       </c>
@@ -10026,7 +10043,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17">
       <c r="A178" s="1">
         <v>161</v>
       </c>
@@ -10075,7 +10092,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17">
       <c r="A179" s="1">
         <v>162</v>
       </c>
@@ -10121,7 +10138,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17">
       <c r="A180" s="1">
         <v>163</v>
       </c>
@@ -10170,7 +10187,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17">
       <c r="A181" s="1">
         <v>164</v>
       </c>
@@ -10216,7 +10233,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17">
       <c r="A182" s="1">
         <v>165</v>
       </c>
@@ -10268,7 +10285,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17">
       <c r="A183" s="1">
         <v>166</v>
       </c>
@@ -10317,7 +10334,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17">
       <c r="A184" s="1">
         <v>167</v>
       </c>
@@ -10366,7 +10383,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17">
       <c r="A185" s="1">
         <v>168</v>
       </c>
@@ -10415,7 +10432,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17">
       <c r="A186" s="1">
         <v>169</v>
       </c>
@@ -10461,7 +10478,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17">
       <c r="A187" s="1">
         <v>170</v>
       </c>
@@ -10516,7 +10533,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17">
       <c r="A188" s="1">
         <v>171</v>
       </c>
@@ -10565,7 +10582,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17">
       <c r="A189" s="1">
         <v>172</v>
       </c>
@@ -10611,7 +10628,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17">
       <c r="A190" s="1">
         <v>173</v>
       </c>
@@ -10657,7 +10674,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17">
       <c r="A191" s="1">
         <v>174</v>
       </c>
@@ -10712,7 +10729,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17">
       <c r="A192" s="1">
         <v>175</v>
       </c>
@@ -10761,7 +10778,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17">
       <c r="A193" s="1">
         <v>176</v>
       </c>
@@ -10807,7 +10824,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17">
       <c r="A194" s="1">
         <v>177</v>
       </c>
@@ -10856,7 +10873,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17">
       <c r="A195" s="1">
         <v>178</v>
       </c>
@@ -10902,7 +10919,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17">
       <c r="A196" s="1">
         <v>179</v>
       </c>
@@ -10957,7 +10974,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17">
       <c r="A197" s="1">
         <v>180</v>
       </c>
@@ -11006,7 +11023,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17">
       <c r="A198" s="1">
         <v>181</v>
       </c>
@@ -11055,7 +11072,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17">
       <c r="A199" s="1">
         <v>182</v>
       </c>
@@ -11101,7 +11118,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17">
       <c r="A200" s="1">
         <v>183</v>
       </c>
@@ -11147,7 +11164,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17">
       <c r="A201" s="1">
         <v>184</v>
       </c>
@@ -11193,7 +11210,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17">
       <c r="A202" s="1">
         <v>185</v>
       </c>
@@ -11248,7 +11265,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17">
       <c r="A203" s="1">
         <v>186</v>
       </c>
@@ -11297,7 +11314,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17">
       <c r="A204" s="1">
         <v>187</v>
       </c>
@@ -11343,7 +11360,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17">
       <c r="A205" s="1">
         <v>188</v>
       </c>
@@ -11389,7 +11406,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17">
       <c r="A206" s="1">
         <v>189</v>
       </c>
@@ -11444,7 +11461,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17">
       <c r="A207" s="1">
         <v>190</v>
       </c>
@@ -11493,7 +11510,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17">
       <c r="A208" s="1">
         <v>191</v>
       </c>
@@ -11539,7 +11556,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17">
       <c r="A209" s="1">
         <v>192</v>
       </c>
@@ -11588,7 +11605,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17">
       <c r="A210" s="1">
         <v>193</v>
       </c>
@@ -11637,7 +11654,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17">
       <c r="A211" s="1">
         <v>194</v>
       </c>
@@ -11683,7 +11700,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17">
       <c r="A212" s="1">
         <v>195</v>
       </c>
@@ -11735,7 +11752,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17">
       <c r="A213" s="1">
         <v>196</v>
       </c>
@@ -11784,7 +11801,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17">
       <c r="A214" s="1">
         <v>197</v>
       </c>
@@ -11833,7 +11850,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17">
       <c r="A215" s="1">
         <v>198</v>
       </c>
@@ -11882,7 +11899,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17">
       <c r="A216" s="1">
         <v>199</v>
       </c>
@@ -11931,7 +11948,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17">
       <c r="A217" s="1">
         <v>200</v>
       </c>
@@ -11977,7 +11994,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17">
       <c r="A218" s="1">
         <v>201</v>
       </c>
@@ -12032,7 +12049,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17">
       <c r="A219" s="1">
         <v>202</v>
       </c>
@@ -12081,7 +12098,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17">
       <c r="A220" s="1">
         <v>203</v>
       </c>
@@ -12127,7 +12144,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17">
       <c r="A221" s="1">
         <v>204</v>
       </c>
@@ -12176,7 +12193,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17">
       <c r="A222" s="1">
         <v>205</v>
       </c>
@@ -12225,7 +12242,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17">
       <c r="A223" s="1">
         <v>206</v>
       </c>
@@ -12271,7 +12288,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17">
       <c r="A224" s="1">
         <v>207</v>
       </c>
@@ -12326,7 +12343,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17">
       <c r="A225" s="1">
         <v>208</v>
       </c>
@@ -12375,7 +12392,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17">
       <c r="A226" s="1">
         <v>209</v>
       </c>
@@ -12421,7 +12438,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17">
       <c r="A227" s="1">
         <v>210</v>
       </c>
@@ -12470,7 +12487,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17">
       <c r="A228" s="1">
         <v>211</v>
       </c>
@@ -12516,7 +12533,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17">
       <c r="A229" s="1">
         <v>212</v>
       </c>
@@ -12562,7 +12579,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17">
       <c r="A230" s="1">
         <v>213</v>
       </c>
@@ -12617,7 +12634,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17">
       <c r="A231" s="1">
         <v>214</v>
       </c>
@@ -12666,7 +12683,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17">
       <c r="A232" s="1">
         <v>215</v>
       </c>
@@ -12715,7 +12732,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17">
       <c r="A233" s="1">
         <v>216</v>
       </c>
@@ -12761,7 +12778,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17">
       <c r="A234" s="1">
         <v>217</v>
       </c>
@@ -12807,7 +12824,7 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17">
       <c r="A235" s="1">
         <v>218</v>
       </c>
@@ -12859,7 +12876,7 @@
         <v/>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17">
       <c r="A236" s="1">
         <v>219</v>
       </c>
@@ -12908,7 +12925,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17">
       <c r="A237" s="1">
         <v>220</v>
       </c>
@@ -12957,7 +12974,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17">
       <c r="A238" s="1">
         <v>221</v>
       </c>
@@ -13006,7 +13023,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17">
       <c r="A239" s="1">
         <v>222</v>
       </c>
@@ -13052,7 +13069,7 @@
         <v/>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17">
       <c r="A240" s="1">
         <v>223</v>
       </c>
@@ -13104,7 +13121,7 @@
         <v/>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17">
       <c r="A241" s="1">
         <v>224</v>
       </c>
@@ -13153,7 +13170,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17">
       <c r="A242" s="1">
         <v>225</v>
       </c>
@@ -13202,7 +13219,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17">
       <c r="A243" s="1">
         <v>226</v>
       </c>
@@ -13251,7 +13268,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17">
       <c r="A244" s="1">
         <v>227</v>
       </c>
@@ -13297,7 +13314,7 @@
         <v/>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17">
       <c r="A245" s="1">
         <v>228</v>
       </c>
@@ -13352,7 +13369,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17">
       <c r="A246" s="1">
         <v>229</v>
       </c>
@@ -13401,7 +13418,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17">
       <c r="A247" s="1">
         <v>230</v>
       </c>
@@ -13447,7 +13464,7 @@
         <v/>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17">
       <c r="A248" s="1">
         <v>231</v>
       </c>
@@ -13496,7 +13513,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17">
       <c r="A249" s="1">
         <v>232</v>
       </c>
@@ -13542,7 +13559,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17">
       <c r="A250" s="1">
         <v>233</v>
       </c>
@@ -13597,7 +13614,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17">
       <c r="A251" s="1">
         <v>234</v>
       </c>
@@ -13646,7 +13663,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17">
       <c r="A252" s="1">
         <v>235</v>
       </c>
@@ -13692,7 +13709,7 @@
         <v/>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17">
       <c r="A253" s="1">
         <v>236</v>
       </c>
@@ -13741,7 +13758,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17">
       <c r="A254" s="1">
         <v>237</v>
       </c>
@@ -13787,7 +13804,7 @@
         <v/>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17">
       <c r="A255" s="1">
         <v>238</v>
       </c>
@@ -13842,7 +13859,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17">
       <c r="A256" s="1">
         <v>239</v>
       </c>
@@ -13891,7 +13908,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17">
       <c r="A257" s="1">
         <v>240</v>
       </c>
@@ -13937,7 +13954,7 @@
         <v/>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17">
       <c r="A258" s="1">
         <v>241</v>
       </c>
@@ -13986,7 +14003,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17">
       <c r="A259" s="1">
         <v>242</v>
       </c>
@@ -14032,7 +14049,7 @@
         <v/>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17">
       <c r="A260" s="1">
         <v>243</v>
       </c>
@@ -14084,7 +14101,7 @@
         <v/>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17">
       <c r="A261" s="1">
         <v>244</v>
       </c>
@@ -14133,7 +14150,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17">
       <c r="A262" s="1">
         <v>245</v>
       </c>
@@ -14182,7 +14199,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17">
       <c r="A263" s="1">
         <v>246</v>
       </c>
@@ -14228,7 +14245,7 @@
         <v/>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17">
       <c r="A264" s="1">
         <v>247</v>
       </c>
@@ -14283,7 +14300,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17">
       <c r="A265" s="1">
         <v>248</v>
       </c>
@@ -14332,7 +14349,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17">
       <c r="A266" s="1">
         <v>249</v>
       </c>
@@ -14378,7 +14395,7 @@
         <v/>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17">
       <c r="A267" s="1">
         <v>250</v>
       </c>
@@ -14433,7 +14450,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17">
       <c r="A268" s="1">
         <v>251</v>
       </c>
@@ -14482,7 +14499,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17">
       <c r="A269" s="1">
         <v>252</v>
       </c>
@@ -14528,7 +14545,7 @@
         <v/>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17">
       <c r="A270" s="1">
         <v>253</v>
       </c>
@@ -14577,7 +14594,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17">
       <c r="A271" s="1">
         <v>254</v>
       </c>
@@ -14626,7 +14643,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17">
       <c r="A272" s="1">
         <v>255</v>
       </c>
@@ -14672,7 +14689,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17">
       <c r="A273" s="1">
         <v>256</v>
       </c>
@@ -14727,7 +14744,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17">
       <c r="A274" s="1">
         <v>257</v>
       </c>
@@ -14776,7 +14793,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17">
       <c r="A275" s="1">
         <v>258</v>
       </c>
@@ -14825,7 +14842,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17">
       <c r="A276" s="1">
         <v>259</v>
       </c>
@@ -14874,7 +14891,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17">
       <c r="A277" s="1">
         <v>260</v>
       </c>
@@ -14920,7 +14937,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17">
       <c r="A278" s="1">
         <v>261</v>
       </c>
@@ -14966,7 +14983,7 @@
         <v/>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17">
       <c r="A279" s="1">
         <v>262</v>
       </c>
@@ -15021,7 +15038,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17">
       <c r="A280" s="1">
         <v>263</v>
       </c>
@@ -15070,7 +15087,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17">
       <c r="A281" s="1">
         <v>264</v>
       </c>
@@ -15116,7 +15133,7 @@
         <v/>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17">
       <c r="A282" s="1">
         <v>265</v>
       </c>
@@ -15165,7 +15182,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17">
       <c r="A283" s="1">
         <v>266</v>
       </c>
@@ -15214,7 +15231,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17">
       <c r="A284" s="1">
         <v>267</v>
       </c>
@@ -15260,7 +15277,7 @@
         <v/>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17">
       <c r="A285" s="1">
         <v>268</v>
       </c>
@@ -15315,7 +15332,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17">
       <c r="A286" s="1">
         <v>269</v>
       </c>
@@ -15364,7 +15381,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17">
       <c r="A287" s="1">
         <v>270</v>
       </c>
@@ -15410,7 +15427,7 @@
         <v/>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17">
       <c r="A288" s="1">
         <v>271</v>
       </c>
@@ -15459,7 +15476,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17">
       <c r="A289" s="1">
         <v>272</v>
       </c>
@@ -15505,7 +15522,7 @@
         <v/>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17">
       <c r="A290" s="1">
         <v>273</v>
       </c>
@@ -15551,7 +15568,7 @@
         <v/>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17">
       <c r="A291" s="1">
         <v>274</v>
       </c>
@@ -15606,7 +15623,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17">
       <c r="A292" s="1">
         <v>275</v>
       </c>
@@ -15655,7 +15672,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17">
       <c r="A293" s="1">
         <v>276</v>
       </c>
@@ -15704,7 +15721,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17">
       <c r="A294" s="1">
         <v>277</v>
       </c>
@@ -15750,7 +15767,7 @@
         <v/>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17">
       <c r="A295" s="1">
         <v>278</v>
       </c>
@@ -15796,7 +15813,7 @@
         <v/>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17">
       <c r="A296" s="1">
         <v>279</v>
       </c>
@@ -15848,7 +15865,7 @@
         <v/>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17">
       <c r="A297" s="1">
         <v>280</v>
       </c>
@@ -15894,7 +15911,7 @@
         <v/>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17">
       <c r="A298" s="1">
         <v>281</v>
       </c>
@@ -15942,7 +15959,7 @@
         <v>Bool</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17">
       <c r="A299" s="1">
         <v>282</v>
       </c>
@@ -15984,7 +16001,7 @@
         <v>Bool</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17">
       <c r="A300" s="1">
         <v>283</v>
       </c>
@@ -16026,7 +16043,7 @@
         <v>Bool</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17">
       <c r="A301" s="1">
         <v>284</v>
       </c>
@@ -16068,7 +16085,7 @@
         <v>Bool</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17">
       <c r="A302" s="1"/>
       <c r="C302" t="s">
         <v>386</v>
@@ -16098,7 +16115,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17">
       <c r="A303" s="1"/>
       <c r="C303" t="s">
         <v>387</v>
@@ -16125,7 +16142,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17">
       <c r="A304" s="1"/>
       <c r="C304" t="s">
         <v>388</v>
@@ -16152,7 +16169,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19">
       <c r="A305" s="1"/>
       <c r="C305" t="s">
         <v>389</v>
@@ -16179,7 +16196,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19">
       <c r="C306" t="s">
         <v>386</v>
       </c>
@@ -16212,7 +16229,7 @@
         <v/>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19">
       <c r="C307" t="s">
         <v>387</v>
       </c>
@@ -16242,7 +16259,7 @@
         <v/>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19">
       <c r="C308" t="s">
         <v>388</v>
       </c>
@@ -16272,7 +16289,7 @@
         <v/>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19">
       <c r="C309" t="s">
         <v>389</v>
       </c>
@@ -16302,7 +16319,7 @@
         <v/>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19">
       <c r="A310" s="1">
         <v>285</v>
       </c>
@@ -16351,7 +16368,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19">
       <c r="A311" s="1">
         <v>286</v>
       </c>
@@ -16397,7 +16414,7 @@
         <v/>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19">
       <c r="A312" s="1">
         <v>287</v>
       </c>
@@ -16443,7 +16460,7 @@
         <v/>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19">
       <c r="A313" s="1">
         <v>288</v>
       </c>
@@ -16489,7 +16506,7 @@
         <v/>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19">
       <c r="A314" s="1">
         <v>289</v>
       </c>
@@ -16535,7 +16552,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19">
       <c r="A315" s="1">
         <v>290</v>
       </c>
@@ -16587,7 +16604,7 @@
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19">
       <c r="A316" s="1">
         <v>291</v>
       </c>
@@ -16636,7 +16653,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19">
       <c r="A317" s="1">
         <v>292</v>
       </c>
@@ -16685,7 +16702,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19">
       <c r="A318" s="1">
         <v>293</v>
       </c>
@@ -16731,7 +16748,7 @@
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19">
       <c r="A319" s="1">
         <v>294</v>
       </c>
@@ -16783,7 +16800,7 @@
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19">
       <c r="A320" s="1">
         <v>295</v>
       </c>
@@ -16832,7 +16849,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17">
       <c r="A321" s="1">
         <v>296</v>
       </c>
@@ -16881,7 +16898,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17">
       <c r="A322" s="1">
         <v>297</v>
       </c>
@@ -16930,7 +16947,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17">
       <c r="A323" s="1">
         <v>298</v>
       </c>
@@ -16976,7 +16993,7 @@
         <v/>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17">
       <c r="A324" s="1">
         <v>299</v>
       </c>
@@ -17028,7 +17045,7 @@
         <v/>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17">
       <c r="A325" s="1">
         <v>300</v>
       </c>
@@ -17077,7 +17094,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17">
       <c r="A326" s="1">
         <v>301</v>
       </c>
@@ -17126,7 +17143,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17">
       <c r="A327" s="1">
         <v>302</v>
       </c>
@@ -17172,7 +17189,7 @@
         <v/>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17">
       <c r="A328" s="1">
         <v>303</v>
       </c>
@@ -17224,7 +17241,7 @@
         <v/>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17">
       <c r="A329" s="1">
         <v>304</v>
       </c>
@@ -17273,7 +17290,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17">
       <c r="A330" s="1">
         <v>305</v>
       </c>
@@ -17319,7 +17336,7 @@
         <v/>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17">
       <c r="A331" s="1">
         <v>306</v>
       </c>
@@ -17365,7 +17382,7 @@
         <v/>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17">
       <c r="A332" s="1">
         <v>307</v>
       </c>
@@ -17414,7 +17431,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17">
       <c r="A333" s="1">
         <v>308</v>
       </c>
@@ -17460,7 +17477,7 @@
         <v/>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17">
       <c r="A334" s="1">
         <v>309</v>
       </c>
@@ -17512,7 +17529,7 @@
         <v/>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17">
       <c r="A335" s="1">
         <v>310</v>
       </c>
@@ -17561,7 +17578,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17">
       <c r="A336" s="1">
         <v>311</v>
       </c>
@@ -17610,7 +17627,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17">
       <c r="A337" s="1">
         <v>312</v>
       </c>
@@ -17656,7 +17673,7 @@
         <v/>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17">
       <c r="A338" s="1">
         <v>313</v>
       </c>
@@ -17708,7 +17725,7 @@
         <v/>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17">
       <c r="A339" s="1">
         <v>314</v>
       </c>
@@ -17757,7 +17774,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17">
       <c r="A340" s="1">
         <v>315</v>
       </c>
@@ -17806,7 +17823,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17">
       <c r="A341" s="1">
         <v>316</v>
       </c>
@@ -17852,7 +17869,7 @@
         <v/>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17">
       <c r="A342" s="1">
         <v>317</v>
       </c>
@@ -17898,7 +17915,7 @@
         <v/>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17">
       <c r="A343" s="1">
         <v>318</v>
       </c>
@@ -17950,7 +17967,7 @@
         <v/>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17">
       <c r="A344" s="1">
         <v>319</v>
       </c>
@@ -17999,7 +18016,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17">
       <c r="A345" s="1">
         <v>320</v>
       </c>
@@ -18045,7 +18062,7 @@
         <v/>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17">
       <c r="A346" s="1">
         <v>321</v>
       </c>
@@ -18094,7 +18111,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17">
       <c r="A347" s="1">
         <v>322</v>
       </c>
@@ -18140,7 +18157,7 @@
         <v/>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17">
       <c r="A348" s="1">
         <v>323</v>
       </c>
@@ -18192,7 +18209,7 @@
         <v/>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17">
       <c r="A349" s="1">
         <v>324</v>
       </c>
@@ -18241,7 +18258,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17">
       <c r="A350" s="1">
         <v>325</v>
       </c>
@@ -18290,7 +18307,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17">
       <c r="A351" s="1">
         <v>326</v>
       </c>
@@ -18339,7 +18356,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17">
       <c r="A352" s="1">
         <v>327</v>
       </c>
@@ -18385,7 +18402,7 @@
         <v/>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17">
       <c r="A353" s="1">
         <v>328</v>
       </c>
@@ -18437,7 +18454,7 @@
         <v/>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17">
       <c r="A354" s="1">
         <v>329</v>
       </c>
@@ -18486,7 +18503,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17">
       <c r="A355" s="1">
         <v>330</v>
       </c>
@@ -18535,7 +18552,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17">
       <c r="A356" s="1">
         <v>331</v>
       </c>
@@ -18581,7 +18598,7 @@
         <v/>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17">
       <c r="A357" s="1">
         <v>332</v>
       </c>
@@ -18633,7 +18650,7 @@
         <v/>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17">
       <c r="A358" s="1">
         <v>333</v>
       </c>
@@ -18682,7 +18699,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17">
       <c r="A359" s="1">
         <v>334</v>
       </c>
@@ -18731,7 +18748,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17">
       <c r="A360" s="1">
         <v>335</v>
       </c>
@@ -18777,7 +18794,7 @@
         <v/>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17">
       <c r="A361" s="1">
         <v>336</v>
       </c>
@@ -18829,7 +18846,7 @@
         <v/>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17">
       <c r="A362" s="1">
         <v>337</v>
       </c>
@@ -18878,7 +18895,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17">
       <c r="A363" s="1">
         <v>338</v>
       </c>
@@ -18927,7 +18944,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17">
       <c r="A364" s="1">
         <v>339</v>
       </c>
@@ -18973,7 +18990,7 @@
         <v/>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17">
       <c r="A365" s="1">
         <v>340</v>
       </c>
@@ -19025,7 +19042,7 @@
         <v/>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17">
       <c r="A366" s="1">
         <v>341</v>
       </c>
@@ -19074,7 +19091,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17">
       <c r="A367" s="1">
         <v>342</v>
       </c>
@@ -19123,7 +19140,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17">
       <c r="A368" s="1">
         <v>343</v>
       </c>
@@ -19169,7 +19186,7 @@
         <v/>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17">
       <c r="A369" s="1">
         <v>344</v>
       </c>
@@ -19221,7 +19238,7 @@
         <v/>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17">
       <c r="A370" s="1">
         <v>345</v>
       </c>
@@ -19270,7 +19287,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:17">
       <c r="A371" s="1">
         <v>346</v>
       </c>
@@ -19316,7 +19333,7 @@
         <v/>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:17">
       <c r="A372" s="1">
         <v>347</v>
       </c>
@@ -19365,7 +19382,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:17">
       <c r="A373" s="1">
         <v>348</v>
       </c>
@@ -19411,7 +19428,7 @@
         <v/>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:17">
       <c r="A374" s="1">
         <v>349</v>
       </c>
@@ -19463,7 +19480,7 @@
         <v/>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17">
       <c r="A375" s="1">
         <v>350</v>
       </c>
@@ -19512,7 +19529,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17">
       <c r="A376" s="1">
         <v>351</v>
       </c>
@@ -19561,7 +19578,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17">
       <c r="A377" s="1">
         <v>352</v>
       </c>
@@ -19607,7 +19624,7 @@
         <v/>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17">
       <c r="A378" s="1">
         <v>353</v>
       </c>
@@ -19659,7 +19676,7 @@
         <v/>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17">
       <c r="A379" s="1">
         <v>354</v>
       </c>
@@ -19708,7 +19725,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17">
       <c r="A380" s="1">
         <v>355</v>
       </c>
@@ -19757,7 +19774,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17">
       <c r="A381" s="1">
         <v>356</v>
       </c>
@@ -19803,7 +19820,7 @@
         <v/>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17">
       <c r="A382" s="1">
         <v>357</v>
       </c>
@@ -19855,7 +19872,7 @@
         <v/>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:17">
       <c r="A383" s="1">
         <v>358</v>
       </c>
@@ -19904,7 +19921,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17">
       <c r="A384" s="1">
         <v>359</v>
       </c>
@@ -19953,7 +19970,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17">
       <c r="A385" s="1">
         <v>360</v>
       </c>
@@ -19999,7 +20016,7 @@
         <v/>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:17">
       <c r="A386" s="1">
         <v>361</v>
       </c>
@@ -20051,7 +20068,7 @@
         <v/>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:17">
       <c r="A387" s="1">
         <v>362</v>
       </c>
@@ -20100,7 +20117,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:17">
       <c r="A388" s="1">
         <v>363</v>
       </c>
@@ -20149,7 +20166,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:17">
       <c r="A389" s="1">
         <v>364</v>
       </c>
@@ -20195,7 +20212,7 @@
         <v/>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:17">
       <c r="A390" s="1">
         <v>365</v>
       </c>
@@ -20246,7 +20263,7 @@
         <v/>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:17">
       <c r="A391" s="1">
         <v>366</v>
       </c>
@@ -20295,7 +20312,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:17">
       <c r="A392" s="1">
         <v>367</v>
       </c>
@@ -20344,7 +20361,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:17">
       <c r="A393" s="1">
         <v>368</v>
       </c>
@@ -20390,7 +20407,7 @@
         <v/>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:17">
       <c r="A394" s="1">
         <v>369</v>
       </c>
@@ -20442,7 +20459,7 @@
         <v/>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:17">
       <c r="A395" s="1">
         <v>370</v>
       </c>
@@ -20491,7 +20508,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17">
       <c r="A396" s="1">
         <v>371</v>
       </c>
@@ -20540,7 +20557,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17">
       <c r="A397" s="1">
         <v>372</v>
       </c>
@@ -20586,7 +20603,7 @@
         <v/>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:17">
       <c r="A398" s="1">
         <v>373</v>
       </c>
@@ -20638,7 +20655,7 @@
         <v/>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:17">
       <c r="A399" s="1">
         <v>374</v>
       </c>
@@ -20687,7 +20704,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:17">
       <c r="A400" s="1">
         <v>375</v>
       </c>
@@ -20736,7 +20753,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:17">
       <c r="A401" s="1">
         <v>376</v>
       </c>
@@ -20782,7 +20799,7 @@
         <v/>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:17">
       <c r="A402" s="1">
         <v>377</v>
       </c>
@@ -20837,7 +20854,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:17">
       <c r="A403" s="1">
         <v>378</v>
       </c>
@@ -20883,7 +20900,7 @@
         <v/>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:17">
       <c r="A404" s="1">
         <v>379</v>
       </c>
@@ -20929,7 +20946,7 @@
         <v/>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:17">
       <c r="A405" s="1">
         <v>380</v>
       </c>
@@ -20981,7 +20998,7 @@
         <v/>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:17">
       <c r="A406" s="1">
         <v>381</v>
       </c>
@@ -21030,7 +21047,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:17">
       <c r="A407" s="1">
         <v>382</v>
       </c>
@@ -21079,7 +21096,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:17">
       <c r="A408" s="1">
         <v>383</v>
       </c>
@@ -21125,7 +21142,7 @@
         <v/>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:17">
       <c r="A409" s="1">
         <v>384</v>
       </c>
@@ -21177,7 +21194,7 @@
         <v/>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:17">
       <c r="A410" s="1">
         <v>385</v>
       </c>
@@ -21226,7 +21243,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:17">
       <c r="A411" s="1">
         <v>386</v>
       </c>
@@ -21272,7 +21289,7 @@
         <v/>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:17">
       <c r="A412" s="1">
         <v>387</v>
       </c>
@@ -21321,7 +21338,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:17">
       <c r="A413" s="1">
         <v>388</v>
       </c>
@@ -21367,7 +21384,7 @@
         <v/>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:17">
       <c r="A414" s="1">
         <v>389</v>
       </c>
@@ -21419,7 +21436,7 @@
         <v/>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:17">
       <c r="A415" s="1">
         <v>390</v>
       </c>
@@ -21468,7 +21485,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:17">
       <c r="A416" s="1">
         <v>391</v>
       </c>
@@ -21517,7 +21534,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:17">
       <c r="A417" s="1">
         <v>392</v>
       </c>
@@ -21563,7 +21580,7 @@
         <v/>
       </c>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:17">
       <c r="A418" s="1">
         <v>393</v>
       </c>
@@ -21615,7 +21632,7 @@
         <v/>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:17">
       <c r="A419" s="1">
         <v>394</v>
       </c>
@@ -21664,7 +21681,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:17">
       <c r="A420" s="1">
         <v>395</v>
       </c>
@@ -21713,7 +21730,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="421" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:17">
       <c r="A421" s="1">
         <v>396</v>
       </c>
@@ -21759,7 +21776,7 @@
         <v/>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:17">
       <c r="A422" s="1">
         <v>397</v>
       </c>
@@ -21805,7 +21822,7 @@
         <v/>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:17">
       <c r="A423" s="1">
         <v>398</v>
       </c>
@@ -21857,7 +21874,7 @@
         <v/>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:17">
       <c r="A424" s="1">
         <v>399</v>
       </c>
@@ -21906,7 +21923,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:17">
       <c r="A425" s="1">
         <v>400</v>
       </c>
@@ -21955,7 +21972,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="426" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:17">
       <c r="A426" s="1">
         <v>401</v>
       </c>
@@ -22001,7 +22018,7 @@
         <v/>
       </c>
     </row>
-    <row r="427" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:17">
       <c r="A427" s="1">
         <v>402</v>
       </c>
@@ -22053,7 +22070,7 @@
         <v/>
       </c>
     </row>
-    <row r="428" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:17">
       <c r="A428" s="1">
         <v>403</v>
       </c>
@@ -22102,7 +22119,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="429" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:17">
       <c r="A429" s="1">
         <v>404</v>
       </c>
@@ -22151,7 +22168,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="430" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:17">
       <c r="A430" s="1">
         <v>405</v>
       </c>
@@ -22197,7 +22214,7 @@
         <v/>
       </c>
     </row>
-    <row r="431" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:17">
       <c r="A431" s="1">
         <v>406</v>
       </c>
@@ -22249,7 +22266,7 @@
         <v/>
       </c>
     </row>
-    <row r="432" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:17">
       <c r="A432" s="1">
         <v>407</v>
       </c>
@@ -22298,7 +22315,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="433" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:17">
       <c r="A433" s="1">
         <v>408</v>
       </c>
@@ -22344,7 +22361,7 @@
         <v/>
       </c>
     </row>
-    <row r="434" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:17">
       <c r="A434" s="1">
         <v>409</v>
       </c>
@@ -22393,7 +22410,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="435" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:17">
       <c r="A435" s="1">
         <v>410</v>
       </c>
@@ -22439,7 +22456,7 @@
         <v/>
       </c>
     </row>
-    <row r="436" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:17">
       <c r="A436" s="1">
         <v>411</v>
       </c>
@@ -22491,7 +22508,7 @@
         <v/>
       </c>
     </row>
-    <row r="437" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:17">
       <c r="A437" s="1">
         <v>412</v>
       </c>
@@ -22540,7 +22557,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="438" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:17">
       <c r="A438" s="1">
         <v>413</v>
       </c>
@@ -22586,7 +22603,7 @@
         <v/>
       </c>
     </row>
-    <row r="439" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:17">
       <c r="A439" s="1">
         <v>414</v>
       </c>
@@ -22635,7 +22652,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="440" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:17">
       <c r="A440" s="1">
         <v>415</v>
       </c>
@@ -22684,7 +22701,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="441" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:17">
       <c r="A441" s="1">
         <v>416</v>
       </c>
@@ -22730,7 +22747,7 @@
         <v/>
       </c>
     </row>
-    <row r="442" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:17">
       <c r="A442" s="1">
         <v>417</v>
       </c>
@@ -22782,7 +22799,7 @@
         <v/>
       </c>
     </row>
-    <row r="443" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:17">
       <c r="A443" s="1">
         <v>418</v>
       </c>
@@ -22831,7 +22848,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="444" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:17">
       <c r="A444" s="1">
         <v>419</v>
       </c>
@@ -22880,7 +22897,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="445" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:17">
       <c r="A445" s="1">
         <v>420</v>
       </c>
@@ -22926,7 +22943,7 @@
         <v/>
       </c>
     </row>
-    <row r="446" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:17">
       <c r="A446" s="1">
         <v>421</v>
       </c>
@@ -22978,7 +22995,7 @@
         <v/>
       </c>
     </row>
-    <row r="447" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:17">
       <c r="A447" s="1">
         <v>422</v>
       </c>
@@ -23027,7 +23044,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="448" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:17">
       <c r="A448" s="1">
         <v>423</v>
       </c>
@@ -23076,7 +23093,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="449" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:17">
       <c r="A449" s="1">
         <v>424</v>
       </c>
@@ -23122,7 +23139,7 @@
         <v/>
       </c>
     </row>
-    <row r="450" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:17">
       <c r="A450" s="1">
         <v>425</v>
       </c>
@@ -23174,7 +23191,7 @@
         <v/>
       </c>
     </row>
-    <row r="451" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:17">
       <c r="A451" s="1">
         <v>426</v>
       </c>
@@ -23223,7 +23240,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="452" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:17">
       <c r="A452" s="1">
         <v>427</v>
       </c>
@@ -23272,7 +23289,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="453" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:17">
       <c r="A453" s="1">
         <v>428</v>
       </c>
@@ -23318,7 +23335,7 @@
         <v/>
       </c>
     </row>
-    <row r="454" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:17">
       <c r="A454" s="1">
         <v>429</v>
       </c>
@@ -23364,7 +23381,7 @@
         <v/>
       </c>
     </row>
-    <row r="455" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:17">
       <c r="A455" s="1">
         <v>430</v>
       </c>
@@ -23416,7 +23433,7 @@
         <v/>
       </c>
     </row>
-    <row r="456" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:17">
       <c r="A456" s="1">
         <v>431</v>
       </c>
@@ -23465,7 +23482,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="457" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:17">
       <c r="A457" s="1">
         <v>432</v>
       </c>
@@ -23514,7 +23531,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="458" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:17">
       <c r="A458" s="1">
         <v>433</v>
       </c>
@@ -23560,7 +23577,7 @@
         <v/>
       </c>
     </row>
-    <row r="459" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:17">
       <c r="A459" s="1">
         <v>434</v>
       </c>
@@ -23612,7 +23629,7 @@
         <v/>
       </c>
     </row>
-    <row r="460" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:17">
       <c r="A460" s="1">
         <v>435</v>
       </c>
@@ -23661,7 +23678,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="461" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:17">
       <c r="A461" s="1">
         <v>436</v>
       </c>
@@ -23710,7 +23727,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="462" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:17">
       <c r="A462" s="1">
         <v>437</v>
       </c>
@@ -23759,7 +23776,7 @@
         <v>fahrenheit</v>
       </c>
     </row>
-    <row r="463" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:17">
       <c r="A463" s="1">
         <v>438</v>
       </c>
@@ -23820,13 +23837,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -23837,7 +23854,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -23845,7 +23862,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated Lists, nothing finalized
</commit_message>
<xml_diff>
--- a/assets/List_AllInputs.xlsx
+++ b/assets/List_AllInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coals01826\Desktop\Coding\hanson-bas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5059EE0D-0B1A-417A-9DAC-D820BA9B5C87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3738D3-F79A-4466-B6BC-C97BE807648C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18615" yWindow="-120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1609,7 +1609,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD22"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>